<commit_message>
Add missing tileset: Shadow
</commit_message>
<xml_diff>
--- a/Project/assets/TilesetsData.xlsx
+++ b/Project/assets/TilesetsData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\Godot_Projects\Git_Hub\mega-man-maker-level-editor\Project\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GodotEngine\MyProj\mega-man-maker-mmlv-editor\Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72ED830E-00DC-4AFF-8B4C-530A46E168CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11310" xr2:uid="{E48CEEC1-E820-4916-AC40-262412BC5E7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11316"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="355">
   <si>
     <t>tileset_filename</t>
   </si>
@@ -198,12 +197,912 @@
   </si>
   <si>
     <t>TstMM3Gemini2</t>
+  </si>
+  <si>
+    <t>TstMM3Gemini3</t>
+  </si>
+  <si>
+    <t>TstMM3Gemini4</t>
+  </si>
+  <si>
+    <t>TstMM3Gemini2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM3Gemini3Animated1</t>
+  </si>
+  <si>
+    <t>TstMM3Gemini4Animated1</t>
+  </si>
+  <si>
+    <t>TstMM3Hard</t>
+  </si>
+  <si>
+    <t>TstMM3Wily1</t>
+  </si>
+  <si>
+    <t>TstMM3Wily1-2</t>
+  </si>
+  <si>
+    <t>TstMM3Wily1-3</t>
+  </si>
+  <si>
+    <t>TstMM3Wily1-3Alt</t>
+  </si>
+  <si>
+    <t>TstMM3Wily2</t>
+  </si>
+  <si>
+    <t>TstMM3Wily3</t>
+  </si>
+  <si>
+    <t>TstMM3Wily4</t>
+  </si>
+  <si>
+    <t>TstMM3Wily4-2</t>
+  </si>
+  <si>
+    <t>TstMM3Wily5</t>
+  </si>
+  <si>
+    <t>TstMM3Wily6</t>
+  </si>
+  <si>
+    <t>TstMM4Ring</t>
+  </si>
+  <si>
+    <t>TstMM4Dive</t>
+  </si>
+  <si>
+    <t>TstMM4DiveAlt</t>
+  </si>
+  <si>
+    <t>TstMM4Skull</t>
+  </si>
+  <si>
+    <t>TstMM4Bright1</t>
+  </si>
+  <si>
+    <t>TstMM4Dust</t>
+  </si>
+  <si>
+    <t>TstMM4Dust2</t>
+  </si>
+  <si>
+    <t>TstMM4Drill</t>
+  </si>
+  <si>
+    <t>TstMM4Drill2</t>
+  </si>
+  <si>
+    <t>TstMM4Toad</t>
+  </si>
+  <si>
+    <t>TstMM4Toad2</t>
+  </si>
+  <si>
+    <t>TstMM4Pharaoh</t>
+  </si>
+  <si>
+    <t>TstMM4Pharaoh2</t>
+  </si>
+  <si>
+    <t>TstMM4Pharaoh3</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack1</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack1-2</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack2</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack3</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack3-2</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack4</t>
+  </si>
+  <si>
+    <t>TstMM4Cossack4-2</t>
+  </si>
+  <si>
+    <t>TstMM4Wily1</t>
+  </si>
+  <si>
+    <t>TstMM4Wily2</t>
+  </si>
+  <si>
+    <t>TstMM4Wily3</t>
+  </si>
+  <si>
+    <t>TstMM4Wily3-2</t>
+  </si>
+  <si>
+    <t>TstMM4Wily4</t>
+  </si>
+  <si>
+    <t>TstMM5Stone</t>
+  </si>
+  <si>
+    <t>TstMM5Stone2</t>
+  </si>
+  <si>
+    <t>TstMM5Gravity</t>
+  </si>
+  <si>
+    <t>TstMM5Crystal1</t>
+  </si>
+  <si>
+    <t>TstMM5CrystalAlt1</t>
+  </si>
+  <si>
+    <t>TstMM5Napalm</t>
+  </si>
+  <si>
+    <t>TstMM5Napalm2</t>
+  </si>
+  <si>
+    <t>TstMM5Gyro</t>
+  </si>
+  <si>
+    <t>TstMM5Star</t>
+  </si>
+  <si>
+    <t>TstMM5Star2</t>
+  </si>
+  <si>
+    <t>TstMM5Star2Alt</t>
+  </si>
+  <si>
+    <t>TstMM5Star3</t>
+  </si>
+  <si>
+    <t>TstMM5Wave1</t>
+  </si>
+  <si>
+    <t>TstMM5Charge</t>
+  </si>
+  <si>
+    <t>TstMM5Charge2</t>
+  </si>
+  <si>
+    <t>TstMM5Dark1</t>
+  </si>
+  <si>
+    <t>TstMM5Dark2</t>
+  </si>
+  <si>
+    <t>TstMM5Dark2-2</t>
+  </si>
+  <si>
+    <t>TstMM5Dark3</t>
+  </si>
+  <si>
+    <t>TstMM5Dark3-2</t>
+  </si>
+  <si>
+    <t>TstMM5Dark4</t>
+  </si>
+  <si>
+    <t>TstMM5Wily1</t>
+  </si>
+  <si>
+    <t>TstMM5Wily1-2</t>
+  </si>
+  <si>
+    <t>TstMM5Wily2</t>
+  </si>
+  <si>
+    <t>TstMM5Wily2Alt</t>
+  </si>
+  <si>
+    <t>TstMM5Wily3</t>
+  </si>
+  <si>
+    <t>TstMM5Wily4</t>
+  </si>
+  <si>
+    <t>TstMM6Blizzard</t>
+  </si>
+  <si>
+    <t>TstMM6Blizzard2</t>
+  </si>
+  <si>
+    <t>TstMM6Wind</t>
+  </si>
+  <si>
+    <t>TstMM6Wind2</t>
+  </si>
+  <si>
+    <t>TstMM6Wind3</t>
+  </si>
+  <si>
+    <t>TstMM6Flame</t>
+  </si>
+  <si>
+    <t>TstMM6Flame2</t>
+  </si>
+  <si>
+    <t>TstMM6Flame3</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk2</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk2Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk3</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk3Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk4</t>
+  </si>
+  <si>
+    <t>TstMM6Tomahawk4Alt</t>
+  </si>
+  <si>
+    <t>TstMM6TomahawkAlt</t>
+  </si>
+  <si>
+    <t>TstMM6Centaur</t>
+  </si>
+  <si>
+    <t>TstMM6Centaur2</t>
+  </si>
+  <si>
+    <t>TstMM6Centaur2Alt</t>
+  </si>
+  <si>
+    <t>TstMM6CentaurAlt</t>
+  </si>
+  <si>
+    <t>TstMM6Knight</t>
+  </si>
+  <si>
+    <t>TstMM6Knight2</t>
+  </si>
+  <si>
+    <t>TstMM6Knight2Alt</t>
+  </si>
+  <si>
+    <t>TstMM6KnightAlt</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato2</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato2Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato3</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato3Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato4</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato4Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato5</t>
+  </si>
+  <si>
+    <t>TstMM6Yamato5Alt</t>
+  </si>
+  <si>
+    <t>TstMM6YamatoAlt</t>
+  </si>
+  <si>
+    <t>TstMM6Plant</t>
+  </si>
+  <si>
+    <t>TstMM6MrX1</t>
+  </si>
+  <si>
+    <t>TstMM6MrX1-2</t>
+  </si>
+  <si>
+    <t>TstMM6MrX2</t>
+  </si>
+  <si>
+    <t>TstMM6MrX2-2</t>
+  </si>
+  <si>
+    <t>TstMM6MrX3</t>
+  </si>
+  <si>
+    <t>TstMM6MrX3Alt</t>
+  </si>
+  <si>
+    <t>TstMM6MrX4</t>
+  </si>
+  <si>
+    <t>TstMM6Wily1</t>
+  </si>
+  <si>
+    <t>TstMM6Wily1Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Wily2</t>
+  </si>
+  <si>
+    <t>TstMM6Wily2Alt</t>
+  </si>
+  <si>
+    <t>TstMM6Wily3</t>
+  </si>
+  <si>
+    <t>TstMM6Wily4</t>
+  </si>
+  <si>
+    <t>MM4</t>
+  </si>
+  <si>
+    <t>MM5</t>
+  </si>
+  <si>
+    <t>MM6</t>
+  </si>
+  <si>
+    <t>MM7</t>
+  </si>
+  <si>
+    <t>TstMM7Spring</t>
+  </si>
+  <si>
+    <t>TstMM7Spring2</t>
+  </si>
+  <si>
+    <t>TstMM7Freeze</t>
+  </si>
+  <si>
+    <t>TstMM7Slash</t>
+  </si>
+  <si>
+    <t>TstMM7Shade2</t>
+  </si>
+  <si>
+    <t>TstMM7Junk</t>
+  </si>
+  <si>
+    <t>TstMM7Shade</t>
+  </si>
+  <si>
+    <t>TstMM7Shade2Alt</t>
+  </si>
+  <si>
+    <t>TstMM7Burst</t>
+  </si>
+  <si>
+    <t>TstMM7Burst2TstMM7Burst3</t>
+  </si>
+  <si>
+    <t>TstMM7Burst3Alt</t>
+  </si>
+  <si>
+    <t>TstMM7Turbo</t>
+  </si>
+  <si>
+    <t>TstMM7Turbo2</t>
+  </si>
+  <si>
+    <t>TstMM7Turbo3</t>
+  </si>
+  <si>
+    <t>TstMM7Turbo4</t>
+  </si>
+  <si>
+    <t>TstMM7Cloud</t>
+  </si>
+  <si>
+    <t>TstMM7Wily1</t>
+  </si>
+  <si>
+    <t>TstMM7Wily2</t>
+  </si>
+  <si>
+    <t>TstMM7Wily3</t>
+  </si>
+  <si>
+    <t>TstMM7Wily4</t>
+  </si>
+  <si>
+    <t>MM8</t>
+  </si>
+  <si>
+    <t>TstMM8Tengu</t>
+  </si>
+  <si>
+    <t>TstMM8Frost</t>
+  </si>
+  <si>
+    <t>TstMM8FrostAlt</t>
+  </si>
+  <si>
+    <t>TstMM8Grenade</t>
+  </si>
+  <si>
+    <t>TstMM8Clown</t>
+  </si>
+  <si>
+    <t>TstMM8Astro2</t>
+  </si>
+  <si>
+    <t>TstMM8Astro2Alt</t>
+  </si>
+  <si>
+    <t>TstMM8Astro</t>
+  </si>
+  <si>
+    <t>TstMM8Sword</t>
+  </si>
+  <si>
+    <t>TstMM8Aqua</t>
+  </si>
+  <si>
+    <t>TstMM8Search</t>
+  </si>
+  <si>
+    <t>TstMM8Wily1</t>
+  </si>
+  <si>
+    <t>TstMM8Wily2</t>
+  </si>
+  <si>
+    <t>TstMM8Wily2Alt</t>
+  </si>
+  <si>
+    <t>MM9</t>
+  </si>
+  <si>
+    <t>TstMM9Concrete</t>
+  </si>
+  <si>
+    <t>TstMM9Concrete2</t>
+  </si>
+  <si>
+    <t>TstMM9Concrete3</t>
+  </si>
+  <si>
+    <t>TstMM9Jewel</t>
+  </si>
+  <si>
+    <t>TstMM9Hornet</t>
+  </si>
+  <si>
+    <t>TstMM9Plug</t>
+  </si>
+  <si>
+    <t>TstMM9Magma</t>
+  </si>
+  <si>
+    <t>TstMM9MagmaTile</t>
+  </si>
+  <si>
+    <t>TstMM9Splash1</t>
+  </si>
+  <si>
+    <t>TstMM9Galaxy</t>
+  </si>
+  <si>
+    <t>TstMM9Tornado</t>
+  </si>
+  <si>
+    <t>TstMM9Tornado2</t>
+  </si>
+  <si>
+    <t>TstMM9Wily1</t>
+  </si>
+  <si>
+    <t>TstMM9Wily1-2</t>
+  </si>
+  <si>
+    <t>TstMM9Wily2Alt1</t>
+  </si>
+  <si>
+    <t>TstMM9Wily2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM9Wily3Animated1</t>
+  </si>
+  <si>
+    <t>TstMM9Wily4Alt1</t>
+  </si>
+  <si>
+    <t>TstMM9Wily4Animated1</t>
+  </si>
+  <si>
+    <t>TstMM9FakeAnimated1</t>
+  </si>
+  <si>
+    <t>TstMM9Fake2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM9Endless</t>
+  </si>
+  <si>
+    <t>TstMM9Endless2</t>
+  </si>
+  <si>
+    <t>TstMM9Endless2Alt</t>
+  </si>
+  <si>
+    <t>TstMM9Endless2Alt2</t>
+  </si>
+  <si>
+    <t>TstMM9Endless3</t>
+  </si>
+  <si>
+    <t>TstMM9Endless3Alt</t>
+  </si>
+  <si>
+    <t>TstMM9Endless4</t>
+  </si>
+  <si>
+    <t>TstMM9Endless4Alt</t>
+  </si>
+  <si>
+    <t>TstMM9Endless5</t>
+  </si>
+  <si>
+    <t>TstMM9Endless6</t>
+  </si>
+  <si>
+    <t>TstMM9Endless7</t>
+  </si>
+  <si>
+    <t>TstMM9Endless8</t>
+  </si>
+  <si>
+    <t>TstMM9Endless8Alt</t>
+  </si>
+  <si>
+    <t>TstMM9Endless9</t>
+  </si>
+  <si>
+    <t>TstMM9Endless9Alt</t>
+  </si>
+  <si>
+    <t>TstMM9Endless10</t>
+  </si>
+  <si>
+    <t>MM10</t>
+  </si>
+  <si>
+    <t>TstMM10Blade</t>
+  </si>
+  <si>
+    <t>TstMM10Blade2</t>
+  </si>
+  <si>
+    <t>TstMM10Solar2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Solar3Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10SolarAnimated1</t>
+  </si>
+  <si>
+    <t>TstMM10Sheep1</t>
+  </si>
+  <si>
+    <t>TstMM10Commando</t>
+  </si>
+  <si>
+    <t>TstMM10Pump</t>
+  </si>
+  <si>
+    <t>TstMM10Pump2</t>
+  </si>
+  <si>
+    <t>TstMM10Pump2Alt</t>
+  </si>
+  <si>
+    <t>TstMM10PumpAlt</t>
+  </si>
+  <si>
+    <t>TstMM10Strike</t>
+  </si>
+  <si>
+    <t>TstMM10Strike2</t>
+  </si>
+  <si>
+    <t>TstMM10Nitro</t>
+  </si>
+  <si>
+    <t>TstMM10Nitro2</t>
+  </si>
+  <si>
+    <t>TstMM10ChillAnimated1</t>
+  </si>
+  <si>
+    <t>TstMM10Chill2</t>
+  </si>
+  <si>
+    <t>TstMM10Wily1</t>
+  </si>
+  <si>
+    <t>TstMM10Wily1-2</t>
+  </si>
+  <si>
+    <t>TstMM10Wily1-3</t>
+  </si>
+  <si>
+    <t>TstMM10Wily1-4</t>
+  </si>
+  <si>
+    <t>TstMM10Wily2</t>
+  </si>
+  <si>
+    <t>TstMM10Wily2-2</t>
+  </si>
+  <si>
+    <t>TstMM10Wily2-3</t>
+  </si>
+  <si>
+    <t>TstMM10Wily3</t>
+  </si>
+  <si>
+    <t>TstMM10Wily3-2</t>
+  </si>
+  <si>
+    <t>TstMM10Wily3-2Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Wily3Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Wily4</t>
+  </si>
+  <si>
+    <t>TstMM10Wily4Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Wily5-2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Wily5-3Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Wily5-4Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Wily5Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Enker</t>
+  </si>
+  <si>
+    <t>TstMM10Enker2</t>
+  </si>
+  <si>
+    <t>TstMM10Enker3</t>
+  </si>
+  <si>
+    <t>TstMM10Enker4</t>
+  </si>
+  <si>
+    <t>TstMM10Enker5</t>
+  </si>
+  <si>
+    <t>TstMM10Enker6</t>
+  </si>
+  <si>
+    <t>TstMM10Punk</t>
+  </si>
+  <si>
+    <t>TstMM10Punk2</t>
+  </si>
+  <si>
+    <t>TstMM10Punk3</t>
+  </si>
+  <si>
+    <t>TstMM10Punk4Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Ballade</t>
+  </si>
+  <si>
+    <t>TstMM10Ballade2</t>
+  </si>
+  <si>
+    <t>TstMM10Endless</t>
+  </si>
+  <si>
+    <t>TstMM10Endless2</t>
+  </si>
+  <si>
+    <t>TstMM10Endless3</t>
+  </si>
+  <si>
+    <t>TstMM10Endless3Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Endless4</t>
+  </si>
+  <si>
+    <t>TstMM10Endless5</t>
+  </si>
+  <si>
+    <t>TstMM10Endless6</t>
+  </si>
+  <si>
+    <t>TstMM10Endless6Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Endless7</t>
+  </si>
+  <si>
+    <t>TstMM10Endless8</t>
+  </si>
+  <si>
+    <t>TstMM10Endless9</t>
+  </si>
+  <si>
+    <t>TstMM10Endless10</t>
+  </si>
+  <si>
+    <t>TstMM10Endless11Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Endless12</t>
+  </si>
+  <si>
+    <t>TstMM10Endless13</t>
+  </si>
+  <si>
+    <t>TstMM10Endless14</t>
+  </si>
+  <si>
+    <t>TstMM10Endless15</t>
+  </si>
+  <si>
+    <t>TstMM10Endless16</t>
+  </si>
+  <si>
+    <t>TstMM10Endless17</t>
+  </si>
+  <si>
+    <t>TstMM10Endless18</t>
+  </si>
+  <si>
+    <t>TstMM10Endless18Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Endless19</t>
+  </si>
+  <si>
+    <t>TstMM10Endless20</t>
+  </si>
+  <si>
+    <t>TstMM10Endless21</t>
+  </si>
+  <si>
+    <t>TstMM10Endless21Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Endless22</t>
+  </si>
+  <si>
+    <t>TstMM10Endless22Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Endless23</t>
+  </si>
+  <si>
+    <t>TstMM10Endless24</t>
+  </si>
+  <si>
+    <t>TstMM10Endless25</t>
+  </si>
+  <si>
+    <t>TstMM10Endless25Alt</t>
+  </si>
+  <si>
+    <t>TstMM10Endless26</t>
+  </si>
+  <si>
+    <t>TstMM10Endless27</t>
+  </si>
+  <si>
+    <t>TstMM10Endless28</t>
+  </si>
+  <si>
+    <t>TstMM10Endless29</t>
+  </si>
+  <si>
+    <t>TstMM10Endless30</t>
+  </si>
+  <si>
+    <t>TstMM10Challenge1Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Challenge1AltAnimated1</t>
+  </si>
+  <si>
+    <t>TstMM10Challenge1Alt2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Challenge2AltAnimated1</t>
+  </si>
+  <si>
+    <t>TstMM10Challenge2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM10Challenge3</t>
+  </si>
+  <si>
+    <t>TstMM10Difficulty</t>
+  </si>
+  <si>
+    <t>MM11</t>
+  </si>
+  <si>
+    <t>TstMM11Block</t>
+  </si>
+  <si>
+    <t>TstMM11Acid</t>
+  </si>
+  <si>
+    <t>TstMM11Blast</t>
+  </si>
+  <si>
+    <t>TstMM11Bounce1</t>
+  </si>
+  <si>
+    <t>TstMM11Tundra</t>
+  </si>
+  <si>
+    <t>TstMM11Impact</t>
+  </si>
+  <si>
+    <t>TstMM11Torch1</t>
+  </si>
+  <si>
+    <t>TstMM11Fuse</t>
+  </si>
+  <si>
+    <t>TstMM11Fuse2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM11Wily1Animated1</t>
+  </si>
+  <si>
+    <t>TstMM11Wily2Alt2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM11Wily2Alt3Animated1</t>
+  </si>
+  <si>
+    <t>TstMM11Wily2AltAnimated1</t>
+  </si>
+  <si>
+    <t>TstMM11Wily2Animated1</t>
+  </si>
+  <si>
+    <t>TstMM11Wily1-2Animated1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,8 +1132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,19 +1448,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AE5473-9B48-4DCC-AF2B-5AD28D24E2F4}">
-  <dimension ref="B2:D52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="D344" sqref="D344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -568,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>41</v>
       </c>
@@ -579,7 +1479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>4</v>
       </c>
@@ -587,7 +1487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>21</v>
       </c>
@@ -595,7 +1495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>23</v>
       </c>
@@ -603,7 +1503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>22</v>
       </c>
@@ -611,7 +1511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>5</v>
       </c>
@@ -619,7 +1519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>477</v>
       </c>
@@ -627,7 +1527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>129</v>
       </c>
@@ -635,7 +1535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>478</v>
       </c>
@@ -643,7 +1543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>130</v>
       </c>
@@ -651,7 +1551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>198</v>
       </c>
@@ -659,7 +1559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>131</v>
       </c>
@@ -667,7 +1567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>167</v>
       </c>
@@ -675,7 +1575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>168</v>
       </c>
@@ -683,7 +1583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>169</v>
       </c>
@@ -691,7 +1591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -702,7 +1602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>199</v>
       </c>
@@ -710,7 +1610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>25</v>
       </c>
@@ -718,7 +1618,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>1</v>
       </c>
@@ -726,7 +1626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>200</v>
       </c>
@@ -734,7 +1634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>26</v>
       </c>
@@ -742,7 +1642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>27</v>
       </c>
@@ -750,7 +1650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>446</v>
       </c>
@@ -758,7 +1658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>447</v>
       </c>
@@ -766,7 +1666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>448</v>
       </c>
@@ -774,7 +1674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>449</v>
       </c>
@@ -782,7 +1682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>450</v>
       </c>
@@ -790,7 +1690,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>28</v>
       </c>
@@ -798,7 +1698,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>29</v>
       </c>
@@ -806,7 +1706,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>201</v>
       </c>
@@ -814,7 +1714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C33">
         <v>457</v>
       </c>
@@ -822,7 +1722,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C34">
         <v>132</v>
       </c>
@@ -830,7 +1730,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>133</v>
       </c>
@@ -838,7 +1738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C36">
         <v>170</v>
       </c>
@@ -846,7 +1746,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C37">
         <v>202</v>
       </c>
@@ -854,7 +1754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>134</v>
       </c>
@@ -862,7 +1762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>203</v>
       </c>
@@ -870,7 +1770,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>135</v>
       </c>
@@ -878,7 +1778,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>42</v>
       </c>
@@ -889,7 +1789,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>31</v>
       </c>
@@ -897,7 +1797,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>435</v>
       </c>
@@ -905,7 +1805,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>32</v>
       </c>
@@ -913,7 +1813,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C45">
         <v>433</v>
       </c>
@@ -921,7 +1821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>33</v>
       </c>
@@ -929,7 +1829,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C47">
         <v>436</v>
       </c>
@@ -937,7 +1837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>204</v>
       </c>
@@ -945,7 +1845,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49">
         <v>34</v>
       </c>
@@ -953,7 +1853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50">
         <v>629</v>
       </c>
@@ -961,7 +1861,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51">
         <v>35</v>
       </c>
@@ -969,7 +1869,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52">
         <v>451</v>
       </c>
@@ -977,7 +1877,1492 @@
         <v>54</v>
       </c>
     </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>172</v>
+      </c>
+      <c r="D69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>173</v>
+      </c>
+      <c r="D95" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D117" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>174</v>
+      </c>
+      <c r="D122" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D125" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D126" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D129" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D130" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D131" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D132" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D133" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D134" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D135" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D136" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D137" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D138" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D139" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D140" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D141" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D142" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D143" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D144" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D145" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D146" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D147" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D148" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D149" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D150" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D151" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D152" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D153" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D154" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D155" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D156" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D157" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D158" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D159" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D160" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D161" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D162" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D163" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D164" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D165" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D166" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D167" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D168" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D169" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>175</v>
+      </c>
+      <c r="D170" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D171" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D172" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D173" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D174" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D175" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D176" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D177" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D178" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D179" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D180" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D181" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D182" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D183" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D184" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D185" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D186" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D187" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D188" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D189" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B190" t="s">
+        <v>196</v>
+      </c>
+      <c r="D190" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D191" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D192" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D193" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D194" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D195" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D196" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D197" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D198" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D199" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D200" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D201" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D202" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D203" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B204" t="s">
+        <v>211</v>
+      </c>
+      <c r="D204" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D205" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D206" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D207" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D208" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D209" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D210" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D211" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D212" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D213" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D214" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D215" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D216" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D217" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D218" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D219" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D220" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D221" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D222" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D223" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D224" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D225" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D226" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D227" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D228" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D229" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D230" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D231" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D232" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D233" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D234" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D235" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D236" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D237" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D238" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D239" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D240" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B241" t="s">
+        <v>249</v>
+      </c>
+      <c r="D241" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D242" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D243" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D244" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D245" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D246" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D247" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D248" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D249" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D250" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D251" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D252" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D253" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D254" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D255" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D256" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D257" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D258" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D259" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D260" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D261" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D262" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D263" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D264" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D265" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D266" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D267" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D268" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D269" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D270" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D271" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D272" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D273" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D274" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D275" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D276" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D277" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D278" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D279" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D280" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D281" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D282" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D283" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D284" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D285" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D286" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D287" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D288" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D289" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D290" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D291" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D292" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D293" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D294" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D295" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D296" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D297" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D298" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D299" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D300" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D301" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D302" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D303" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D304" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D305" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D306" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D307" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D308" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D309" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D310" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D311" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D312" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D313" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D314" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D315" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D316" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D317" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D318" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D319" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D320" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="321" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D321" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="322" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D322" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="323" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D323" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="324" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D324" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="325" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D325" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D326" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D327" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="328" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D328" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="329" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D329" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="330" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B330" t="s">
+        <v>339</v>
+      </c>
+      <c r="D330" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="331" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D331" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="332" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D332" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="333" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D333" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="334" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D334" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="335" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D335" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="336" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D336" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D337" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D338" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D339" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D340" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D341" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D342" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D343" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D344" t="s">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>